<commit_message>
Add marketing website (Sphair), cycle tracking system, error handling improvements, and UI enhancements
- Added professional marketing website in Sphair/ folder with red/blue branding
- Implemented cycle tracking for Grass Cutting and Panel Washing with historical data
- Improved error messages to be user-friendly and transparent
- Enhanced Dashboard with logo animation and improved UI
- Updated inventory management with duplicate prevention and validation
- Added cycle information to PDF reports
- Prevented selection of completed trackers on Plant page
- Updated README with comprehensive system documentation
</commit_message>
<xml_diff>
--- a/server/templates/excel/CCTV-Annual.xlsx
+++ b/server/templates/excel/CCTV-Annual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PJs\ChecksheetsApp\server\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732B943E-ED87-41BE-8D67-C0FC5C2750A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC65D8ED-749E-434C-B1EA-5275AA208F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{23D905F4-DE27-4599-B91F-89298AA45371}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Preventive Maintenance Check List</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>PM-017</t>
+  </si>
+  <si>
+    <t>{last_revision_approved_by}</t>
+  </si>
+  <si>
+    <t>{checklist_made_by}</t>
   </si>
 </sst>
 </file>
@@ -1040,6 +1046,105 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1098,105 +1203,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1602,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62187193-A6D8-4851-8C0D-337027B07073}">
   <dimension ref="A1:AF287"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="80" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1"/>
@@ -1634,22 +1640,22 @@
       <c r="C1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="104"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136"/>
+      <c r="S1" s="137"/>
     </row>
     <row r="2" spans="1:21" ht="14.1" customHeight="1" thickTop="1">
       <c r="A2" s="5" t="s">
@@ -1679,29 +1685,29 @@
       <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:21" ht="22.15" customHeight="1" thickBot="1">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="138" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="108" t="s">
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="110"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="142"/>
+      <c r="O3" s="142"/>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="142"/>
+      <c r="R3" s="142"/>
+      <c r="S3" s="143"/>
     </row>
     <row r="4" spans="1:21" ht="14.1" customHeight="1" thickTop="1">
       <c r="A4" s="16"/>
@@ -1731,31 +1737,31 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:21" ht="22.15" customHeight="1" thickBot="1">
-      <c r="A5" s="111" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="111" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="112"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="114" t="s">
+      <c r="A5" s="144" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="144" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="145"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="114"/>
-      <c r="S5" s="115"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="148"/>
     </row>
     <row r="6" spans="1:21" ht="40.15" customHeight="1" thickTop="1">
       <c r="A6" s="21"/>
@@ -1817,11 +1823,11 @@
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1">
       <c r="A8" s="35"/>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="31" t="s">
         <v>44</v>
       </c>
@@ -1877,17 +1883,17 @@
       <c r="G10" s="48"/>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
-      <c r="J10" s="97" t="s">
+      <c r="J10" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="98"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="134"/>
-      <c r="N10" s="134"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
-      <c r="Q10" s="134"/>
-      <c r="R10" s="135"/>
+      <c r="K10" s="131"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="118"/>
+      <c r="R10" s="119"/>
       <c r="S10" s="50"/>
     </row>
     <row r="11" spans="1:21" ht="18.600000000000001" customHeight="1" thickBot="1">
@@ -1900,17 +1906,17 @@
       <c r="G11" s="53"/>
       <c r="H11" s="53"/>
       <c r="I11" s="52"/>
-      <c r="J11" s="117" t="s">
+      <c r="J11" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="138"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+      <c r="R11" s="122"/>
       <c r="S11" s="54"/>
     </row>
     <row r="12" spans="1:21" ht="22.15" customHeight="1">
@@ -1918,28 +1924,28 @@
       <c r="B12" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="99" t="s">
+      <c r="C12" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="128" t="s">
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="129"/>
-      <c r="L12" s="130" t="s">
+      <c r="K12" s="113"/>
+      <c r="L12" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="131"/>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="131"/>
-      <c r="R12" s="132"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="115"/>
+      <c r="P12" s="115"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="116"/>
       <c r="S12" s="56"/>
     </row>
     <row r="13" spans="1:21" ht="19.899999999999999" customHeight="1">
@@ -1954,8 +1960,8 @@
       <c r="G13" s="60"/>
       <c r="H13" s="60"/>
       <c r="I13" s="61"/>
-      <c r="J13" s="147"/>
-      <c r="K13" s="148"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="99"/>
       <c r="L13" s="62"/>
       <c r="M13" s="62"/>
       <c r="N13" s="62"/>
@@ -1970,24 +1976,24 @@
       <c r="B14" s="64">
         <v>1</v>
       </c>
-      <c r="C14" s="142" t="s">
+      <c r="C14" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="143"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="143"/>
-      <c r="I14" s="144"/>
-      <c r="J14" s="145"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
-      <c r="O14" s="120"/>
-      <c r="P14" s="120"/>
-      <c r="Q14" s="120"/>
-      <c r="R14" s="121"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="105"/>
       <c r="S14" s="56"/>
     </row>
     <row r="15" spans="1:21" ht="21" customHeight="1">
@@ -1995,24 +2001,24 @@
       <c r="B15" s="64">
         <v>2</v>
       </c>
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="140"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="140"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="140"/>
-      <c r="I15" s="141"/>
-      <c r="J15" s="145"/>
-      <c r="K15" s="146"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="123"/>
-      <c r="O15" s="123"/>
-      <c r="P15" s="123"/>
-      <c r="Q15" s="123"/>
-      <c r="R15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="108"/>
       <c r="S15" s="56"/>
       <c r="U15" s="65"/>
     </row>
@@ -2021,24 +2027,24 @@
       <c r="B16" s="64">
         <v>3</v>
       </c>
-      <c r="C16" s="139" t="s">
+      <c r="C16" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="140"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="145"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="122"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="124"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="108"/>
       <c r="S16" s="56"/>
     </row>
     <row r="17" spans="1:21" ht="21" customHeight="1">
@@ -2046,24 +2052,24 @@
       <c r="B17" s="64">
         <v>4</v>
       </c>
-      <c r="C17" s="139" t="s">
+      <c r="C17" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="140"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="145"/>
-      <c r="K17" s="146"/>
-      <c r="L17" s="122"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="123"/>
-      <c r="Q17" s="123"/>
-      <c r="R17" s="124"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="107"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="108"/>
       <c r="S17" s="56"/>
       <c r="U17" s="65"/>
     </row>
@@ -2072,24 +2078,24 @@
       <c r="B18" s="64">
         <v>5</v>
       </c>
-      <c r="C18" s="139" t="s">
+      <c r="C18" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="145"/>
-      <c r="K18" s="146"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="123"/>
-      <c r="O18" s="123"/>
-      <c r="P18" s="123"/>
-      <c r="Q18" s="123"/>
-      <c r="R18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="107"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="108"/>
       <c r="S18" s="56"/>
       <c r="U18" s="65"/>
     </row>
@@ -2098,24 +2104,24 @@
       <c r="B19" s="64">
         <v>6</v>
       </c>
-      <c r="C19" s="139" t="s">
+      <c r="C19" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="140"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="145"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="123"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="123"/>
-      <c r="Q19" s="123"/>
-      <c r="R19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="107"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="108"/>
       <c r="S19" s="56"/>
       <c r="U19" s="65"/>
     </row>
@@ -2124,24 +2130,24 @@
       <c r="B20" s="64">
         <v>7</v>
       </c>
-      <c r="C20" s="139" t="s">
+      <c r="C20" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="140"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="146"/>
-      <c r="L20" s="122"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="123"/>
-      <c r="O20" s="123"/>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="124"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="106"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="107"/>
+      <c r="O20" s="107"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="108"/>
       <c r="S20" s="56"/>
     </row>
     <row r="21" spans="1:21" ht="21" customHeight="1">
@@ -2149,24 +2155,24 @@
       <c r="B21" s="64">
         <v>8</v>
       </c>
-      <c r="C21" s="139" t="s">
+      <c r="C21" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="145"/>
-      <c r="K21" s="146"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="126"/>
-      <c r="N21" s="126"/>
-      <c r="O21" s="126"/>
-      <c r="P21" s="126"/>
-      <c r="Q21" s="126"/>
-      <c r="R21" s="127"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="124"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="96"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
+      <c r="O21" s="110"/>
+      <c r="P21" s="110"/>
+      <c r="Q21" s="110"/>
+      <c r="R21" s="111"/>
       <c r="S21" s="56"/>
     </row>
     <row r="22" spans="1:21" ht="2.4500000000000002" customHeight="1">
@@ -2338,13 +2344,13 @@
     </row>
     <row r="31" spans="1:21" ht="21.75" customHeight="1">
       <c r="A31" s="51"/>
-      <c r="B31" s="116" t="s">
+      <c r="B31" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
       <c r="G31" s="76"/>
       <c r="H31" s="77"/>
       <c r="I31" s="77" t="s">
@@ -3069,13 +3075,15 @@
     <row r="287" ht="14.65" customHeight="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="F1:S1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:S3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:S5"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L14:R21"/>
@@ -3092,15 +3100,13 @@
     <mergeCell ref="C19:I19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="F1:S1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:S3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:S5"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nombre del Representante Legal de la Interventoría o Director de Proyecto." sqref="S115:S116 B31 H31:P31" xr:uid="{5E072950-6AE4-4CE2-BF90-B908B97149F1}"/>

</xml_diff>